<commit_message>
actualizacion libro de excel
</commit_message>
<xml_diff>
--- a/Excel/Libro de excel - Casos de prueba - Luisa Fernanda Espinal y Jose Manuel Jaramillo   .xlsx
+++ b/Excel/Libro de excel - Casos de prueba - Luisa Fernanda Espinal y Jose Manuel Jaramillo   .xlsx
@@ -1,17 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27932"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\b12s308\Desktop\cdl\CalculadoraAhorroProgramado\Excel\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DE9132F-F074-4A6D-A1EF-A1A93B5B0A50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Hoja 1" sheetId="1" r:id="rId5"/>
+    <sheet name="Hoja 1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
+      <xlwcv:version setVersion="1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="24">
   <si>
     <t>ENTRADAS</t>
   </si>
@@ -74,42 +99,57 @@
   </si>
   <si>
     <t>Error: abono supera meta de ahorro</t>
+  </si>
+  <si>
+    <t>Mes de Abono Extra</t>
+  </si>
+  <si>
+    <t>Mes de extra superior</t>
+  </si>
+  <si>
+    <t>Error: El Mes en el que se realiza el abono extra es superior al plazo del ahorro</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
-    <font/>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -124,28 +164,40 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
-    <border/>
+  <borders count="10">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
+      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-    </border>
-    <border>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-    </border>
-    <border>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
@@ -155,6 +207,7 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -169,69 +222,164 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf borderId="2" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="3" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="4" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="1" numFmtId="2" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="1" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="2" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+  <cellXfs count="29">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
@@ -239,7 +387,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -429,265 +577,323 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A2:F17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G26" sqref="A4:G26"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="21.0"/>
-    <col customWidth="1" min="2" max="2" width="15.25"/>
-    <col customWidth="1" min="3" max="3" width="13.5"/>
-    <col customWidth="1" min="4" max="4" width="12.88"/>
-    <col customWidth="1" min="5" max="5" width="34.88"/>
+    <col min="1" max="1" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" customWidth="1"/>
+    <col min="5" max="5" width="34.85546875" customWidth="1"/>
+    <col min="6" max="6" width="71.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
-      <c r="B2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="5" t="s">
+      <c r="B2" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="13"/>
+      <c r="D2" s="14"/>
+      <c r="F2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="6" t="s">
+    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" s="17" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="9" t="s">
+    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="10">
-        <v>1100000.0</v>
-      </c>
-      <c r="C4" s="9">
-        <v>6.0</v>
-      </c>
-      <c r="D4" s="11">
-        <v>0.0</v>
-      </c>
-      <c r="E4" s="12">
-        <f t="shared" ref="E4:E6" si="1">(B4-D4)/C4</f>
-        <v>183333.3333</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="9" t="s">
+      <c r="B4" s="7">
+        <v>1100000</v>
+      </c>
+      <c r="C4" s="6">
+        <v>6</v>
+      </c>
+      <c r="D4" s="16">
+        <v>0</v>
+      </c>
+      <c r="E4" s="20">
+        <v>0</v>
+      </c>
+      <c r="F4" s="18">
+        <f>(B4-D4)/C4</f>
+        <v>183333.33333333334</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="10">
-        <v>9000000.0</v>
-      </c>
-      <c r="C5" s="9">
-        <v>12.0</v>
-      </c>
-      <c r="D5" s="11">
-        <v>0.0</v>
-      </c>
-      <c r="E5" s="12">
-        <f t="shared" si="1"/>
+      <c r="B5" s="7">
+        <v>9000000</v>
+      </c>
+      <c r="C5" s="6">
+        <v>12</v>
+      </c>
+      <c r="D5" s="16">
+        <v>0</v>
+      </c>
+      <c r="E5" s="20">
+        <v>0</v>
+      </c>
+      <c r="F5" s="18">
+        <f>(B5-D5)/C5</f>
         <v>750000</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" s="9" t="s">
+    <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="10">
-        <v>1.7E8</v>
-      </c>
-      <c r="C6" s="9">
-        <v>36.0</v>
-      </c>
-      <c r="D6" s="11">
-        <v>0.0</v>
-      </c>
-      <c r="E6" s="12">
-        <f t="shared" si="1"/>
-        <v>4722222.222</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="13"/>
-      <c r="B7" s="13"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="15"/>
-    </row>
-    <row r="8">
-      <c r="A8" s="6" t="s">
+      <c r="B6" s="7">
+        <v>170000000</v>
+      </c>
+      <c r="C6" s="6">
+        <v>36</v>
+      </c>
+      <c r="D6" s="16">
+        <v>0</v>
+      </c>
+      <c r="E6" s="20">
+        <v>0</v>
+      </c>
+      <c r="F6" s="18">
+        <f>(B6-D6)/C6</f>
+        <v>4722222.222222222</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="8"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="9"/>
+      <c r="F7" s="10"/>
+    </row>
+    <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D8" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="E8" s="8" t="s">
+      <c r="E8" s="20"/>
+      <c r="F8" s="17" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" s="9" t="s">
+    <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="10">
-        <v>0.0</v>
-      </c>
-      <c r="C9" s="9">
-        <v>1.0</v>
-      </c>
-      <c r="D9" s="11">
-        <v>0.0</v>
-      </c>
-      <c r="E9" s="12">
-        <f t="shared" ref="E9:E11" si="2">(B9-D9)/C9</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="9" t="s">
+      <c r="B9" s="7">
+        <v>0</v>
+      </c>
+      <c r="C9" s="6">
+        <v>1</v>
+      </c>
+      <c r="D9" s="16">
+        <v>0</v>
+      </c>
+      <c r="E9" s="20">
+        <v>0</v>
+      </c>
+      <c r="F9" s="18">
+        <f>(B9-D9)/C9</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="10">
-        <v>90000.0</v>
-      </c>
-      <c r="C10" s="9">
-        <v>1.0</v>
-      </c>
-      <c r="D10" s="11">
-        <v>0.0</v>
-      </c>
-      <c r="E10" s="12">
-        <f t="shared" si="2"/>
+      <c r="B10" s="7">
         <v>90000</v>
       </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="16" t="s">
+      <c r="C10" s="6">
+        <v>1</v>
+      </c>
+      <c r="D10" s="16">
+        <v>0</v>
+      </c>
+      <c r="E10" s="20">
+        <v>0</v>
+      </c>
+      <c r="F10" s="18">
+        <f>(B10-D10)/C10</f>
+        <v>90000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="10">
-        <v>400000.0</v>
-      </c>
-      <c r="C11" s="9">
-        <v>2.0</v>
-      </c>
-      <c r="D11" s="11">
-        <v>400000.0</v>
-      </c>
-      <c r="E11" s="12">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="13"/>
-      <c r="B12" s="13"/>
-      <c r="C12" s="13"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="15"/>
-    </row>
-    <row r="13">
-      <c r="A13" s="6" t="s">
+      <c r="B11" s="7">
+        <v>400000</v>
+      </c>
+      <c r="C11" s="6">
+        <v>2</v>
+      </c>
+      <c r="D11" s="16">
+        <v>400000</v>
+      </c>
+      <c r="E11" s="20">
+        <v>1</v>
+      </c>
+      <c r="F11" s="18">
+        <f>(B11-D11)/C11</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="8"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="9"/>
+      <c r="F12" s="10"/>
+    </row>
+    <row r="13" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="C13" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="D13" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="E13" s="8" t="s">
+      <c r="E13" s="20"/>
+      <c r="F13" s="17" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" s="9" t="s">
+    <row r="14" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="10">
-        <v>-1300000.0</v>
-      </c>
-      <c r="C14" s="9">
-        <v>15.0</v>
-      </c>
-      <c r="D14" s="11">
-        <v>0.0</v>
-      </c>
-      <c r="E14" s="12" t="s">
+      <c r="B14" s="7">
+        <v>-1300000</v>
+      </c>
+      <c r="C14" s="6">
+        <v>15</v>
+      </c>
+      <c r="D14" s="16">
+        <v>0</v>
+      </c>
+      <c r="E14" s="20">
+        <v>0</v>
+      </c>
+      <c r="F14" s="18" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="15">
-      <c r="A15" s="9" t="s">
+    <row r="15" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="10">
-        <v>50000.0</v>
-      </c>
-      <c r="C15" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="D15" s="11">
-        <v>0.0</v>
-      </c>
-      <c r="E15" s="12" t="s">
+      <c r="B15" s="7">
+        <v>50000</v>
+      </c>
+      <c r="C15" s="6">
+        <v>0</v>
+      </c>
+      <c r="D15" s="16">
+        <v>0</v>
+      </c>
+      <c r="E15" s="20">
+        <v>0</v>
+      </c>
+      <c r="F15" s="18" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="16">
-      <c r="A16" s="9" t="s">
+    <row r="16" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="10">
-        <v>400000.0</v>
-      </c>
-      <c r="C16" s="9">
-        <v>2.0</v>
-      </c>
-      <c r="D16" s="11">
-        <v>800000.0</v>
-      </c>
-      <c r="E16" s="12" t="s">
+      <c r="B16" s="22">
+        <v>400000</v>
+      </c>
+      <c r="C16" s="21">
+        <v>2</v>
+      </c>
+      <c r="D16" s="23">
+        <v>800000</v>
+      </c>
+      <c r="E16" s="25">
+        <v>0</v>
+      </c>
+      <c r="F16" s="26" t="s">
         <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" s="20">
+        <v>200000</v>
+      </c>
+      <c r="C17" s="20">
+        <v>3</v>
+      </c>
+      <c r="D17" s="20">
+        <v>20000</v>
+      </c>
+      <c r="E17" s="27">
+        <v>4</v>
+      </c>
+      <c r="F17" s="28" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:D2"/>
   </mergeCells>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>